<commit_message>
add additional calcs to provide test cases to jasmine
</commit_message>
<xml_diff>
--- a/MonthlyPayments_calcSheet.xlsx
+++ b/MonthlyPayments_calcSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandywoodbury/Dropbox/SoftwareEngineering/Springboard/7.1_JasmineExercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DAEBD8B-E068-4A46-865D-9549F7B36932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A14D461-0148-0245-AFE4-DAC425294ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="12040" windowHeight="16440" xr2:uid="{590112D9-2982-1348-BF21-C36414D0FE71}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Monthly Payments</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>initial values</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>test 3</t>
   </si>
 </sst>
 </file>
@@ -125,7 +137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -139,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -455,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1980C019-899D-F04A-A804-52EEC8020732}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,14 +482,30 @@
     <col min="2" max="2" width="4.1640625" customWidth="1"/>
     <col min="3" max="3" width="2.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -482,8 +513,25 @@
         <f>(D5*D6)/(1-(1+D6)^(-D7))</f>
         <v>1157.788978930311</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="3">
+        <f>(E5*E6)/(1-(1+E6)^(-E7))</f>
+        <v>690.58164027799978</v>
+      </c>
+      <c r="F3" s="3">
+        <f>(F5*F6)/(1-(1+F6)^(-F7))</f>
+        <v>5250.8862015052773</v>
+      </c>
+      <c r="G3" s="3">
+        <f>(G5*G6)/(1-(1+G6)^(-G7))</f>
+        <v>52.085939712494024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -497,8 +545,20 @@
         <f>D10</f>
         <v>250000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="4">
+        <f>E10</f>
+        <v>100000</v>
+      </c>
+      <c r="F5" s="4">
+        <f>F10</f>
+        <v>500000</v>
+      </c>
+      <c r="G5" s="4">
+        <f>G10</f>
+        <v>12500.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -512,8 +572,20 @@
         <f>D12/100/12</f>
         <v>3.1249999999999997E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="5">
+        <f>E12/100/12</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F6" s="5">
+        <f>F12/100/12</f>
+        <v>3.9875000000000006E-3</v>
+      </c>
+      <c r="G6" s="5">
+        <f>G12/100/12</f>
+        <v>8.3333333333333325E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -527,13 +599,33 @@
         <f>D11*12</f>
         <v>360</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="5">
+        <f>E11*12</f>
+        <v>180</v>
+      </c>
+      <c r="F7" s="5">
+        <f>F11*12</f>
+        <v>120</v>
+      </c>
+      <c r="G7" s="5">
+        <f>G11*12</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -543,8 +635,17 @@
       <c r="D10" s="4">
         <v>250000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="4">
+        <v>100000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>500000</v>
+      </c>
+      <c r="G10" s="6">
+        <v>12500.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -554,8 +655,17 @@
       <c r="D11" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="5">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -564,6 +674,15 @@
       </c>
       <c r="D12" s="5">
         <v>3.75</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4.7850000000000001</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>